<commit_message>
Update advance sumary report
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/AdvanceSumaryTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/AdvanceSumaryTemplate.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\workspace\ael\src\main\resources\ExportTemplate\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="12315" windowHeight="8700"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng hợp công nợ nhân viên" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="125725" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>CÔNG TY TNHH TM &amp; DV AEL</t>
   </si>
@@ -108,14 +103,23 @@
     <t>${totalRefAfter}</t>
   </si>
   <si>
-    <t xml:space="preserve">Từ ngày đến ngày </t>
+    <t xml:space="preserve">Từ ngày ${startDate} đến ngày ${endDate} </t>
+  </si>
+  <si>
+    <t>Kế toán trưởng</t>
+  </si>
+  <si>
+    <t>Giám đốc</t>
+  </si>
+  <si>
+    <t>(Ký, họ tên, đóng dấu)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="14">
     <font>
       <sz val="8"/>
       <color indexed="8"/>
@@ -314,6 +318,26 @@
       <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
@@ -322,10 +346,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
@@ -339,22 +359,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
@@ -486,7 +490,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -518,10 +522,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -553,7 +556,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -729,14 +731,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H15" sqref="H15:I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9.5" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" style="3" customWidth="1"/>
@@ -749,98 +751,98 @@
     <col min="9" max="9" width="17.1640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-    </row>
-    <row r="2" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="18" t="s">
+    <row r="1" spans="1:9" ht="15.4" customHeight="1">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" ht="16.149999999999999" customHeight="1">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="18" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.4" customHeight="1">
+      <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-    </row>
-    <row r="4" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-    </row>
-    <row r="5" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="19" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" spans="1:9" ht="16.149999999999999" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="22.15" customHeight="1">
+      <c r="B5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="17" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.4" customHeight="1">
+      <c r="B6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-    </row>
-    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" customHeight="1">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" ht="6" customHeight="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" ht="28.5">
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
@@ -866,7 +868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="18.75" customHeight="1">
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -892,7 +894,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="27.75" customHeight="1">
       <c r="B11" s="5"/>
       <c r="C11" s="8" t="s">
         <v>16</v>
@@ -916,11 +918,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="s">
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="27.75" customHeight="1">
+      <c r="B12" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="7" t="s">
         <v>23</v>
       </c>
@@ -940,90 +942,89 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-    </row>
-    <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="14" t="s">
+    <row r="13" spans="1:9" ht="25.5" customHeight="1">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" ht="18.75" customHeight="1">
+      <c r="B14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-    </row>
-    <row r="15" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="15" t="s">
+      <c r="C14" s="18"/>
+      <c r="E14" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="H14" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="18"/>
+    </row>
+    <row r="15" spans="1:9" ht="18.75" customHeight="1">
+      <c r="B15" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-    </row>
-    <row r="16" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-    </row>
-    <row r="17" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="18" spans="1:9" ht="409.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="12">
+      <c r="C15" s="19"/>
+      <c r="E15" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="19"/>
+      <c r="H15" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="19"/>
+    </row>
+    <row r="16" spans="1:9" ht="63.75" customHeight="1">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" ht="22.15" customHeight="1">
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+    </row>
+    <row r="18" spans="1:9" ht="409.6" customHeight="1">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.4" customHeight="1">
+      <c r="B19" s="16">
         <v>2</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="A18:I18"/>
     <mergeCell ref="B19:I19"/>
@@ -1038,6 +1039,15 @@
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="A13:I13"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
bỏ 2 số thập phân đằng sau tiền (VND ko cần tới thập phân). Giữ lại duy nhất một chỗ là debit của Triển lãm (vì dùng USD). Fix cho toàn bộ UI & export excel Export Excel: ở những chỗ có in ra số tiền bằng chữ, thêm 1 label "Số tiền bằng chữ"
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/AdvanceSumaryTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/AdvanceSumaryTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\src\main\resources\ExportTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Java\ael\src\main\resources\ExportTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="12315" windowHeight="8700"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="12320" windowHeight="8700"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng hợp công nợ nhân viên" sheetId="1" r:id="rId1"/>
@@ -124,9 +124,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.00;[Red]#,##0.00"/>
-  </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
@@ -138,7 +135,7 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <charset val="204"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -314,8 +311,24 @@
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -326,10 +339,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
@@ -346,27 +355,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
@@ -745,114 +742,114 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="18" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="20" style="3" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" style="3" customWidth="1"/>
     <col min="8" max="8" width="20" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="16" t="s">
+    <row r="1" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="16" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-    </row>
-    <row r="4" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="17" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="15" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-    </row>
-    <row r="8" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" ht="28" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
@@ -878,7 +875,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -904,146 +901,137 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="7" t="s">
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="6" t="s">
+      <c r="C12" s="12"/>
+      <c r="D12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="12" t="s">
+    <row r="13" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="E14" s="12" t="s">
+      <c r="C14" s="15"/>
+      <c r="E14" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="H14" s="12" t="s">
+      <c r="F14" s="15"/>
+      <c r="H14" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="13" t="s">
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="E15" s="13" t="s">
+      <c r="C15" s="16"/>
+      <c r="E15" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="H15" s="13" t="s">
+      <c r="F15" s="16"/>
+      <c r="H15" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="13"/>
-    </row>
-    <row r="16" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-    </row>
-    <row r="18" spans="1:9" ht="409.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="10">
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="1:9" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="13">
         <v>2</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="A18:I18"/>
     <mergeCell ref="B19:I19"/>
@@ -1058,6 +1046,15 @@
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="A13:I13"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
change font to Calibri
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/AdvanceSumaryTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/AdvanceSumaryTemplate.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Java\ael\src\main\resources\ExportTemplate\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="12320" windowHeight="8700"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14025" windowHeight="2580"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng hợp công nợ nhân viên" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" calcMode="manual"/>
+  <calcPr calcId="0" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -124,7 +119,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color indexed="8"/>
@@ -132,89 +127,43 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <sz val="12"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <i/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -286,84 +235,72 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
@@ -495,7 +432,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -530,7 +467,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -742,79 +679,80 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20" style="3" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="19.77734375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="20" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="10" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="18" style="10" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="20" style="10" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="20" style="10" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" style="10" customWidth="1"/>
+    <col min="10" max="16384" width="9.33203125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
@@ -829,206 +767,206 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" ht="28" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="4">
         <v>2</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="4">
         <v>3</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="4">
         <v>4</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="4">
         <v>5</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="5"/>
-      <c r="C11" s="17" t="s">
+    <row r="11" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="11" t="s">
+    <row r="12" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="19" t="s">
+      <c r="C12" s="7"/>
+      <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="E14" s="15" t="s">
+      <c r="C14" s="11"/>
+      <c r="E14" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="H14" s="15" t="s">
+      <c r="F14" s="11"/>
+      <c r="H14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="15"/>
+      <c r="I14" s="11"/>
     </row>
     <row r="15" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="E15" s="16" t="s">
+      <c r="C15" s="15"/>
+      <c r="E15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="H15" s="16" t="s">
+      <c r="F15" s="15"/>
+      <c r="H15" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="16"/>
+      <c r="I15" s="15"/>
     </row>
     <row r="16" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
     </row>
     <row r="18" spans="1:9" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="13">
+      <c r="B19" s="16">
         <v>2</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>